<commit_message>
Changed to match MA1
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
+++ b/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan Mercer\Google Drive\  QR\  Videos\Tech\Unit 2\Unit 2 Tech Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\Offline\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF973B77-54C8-4AED-A240-BF1CC3A75B58}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="10020"/>
+    <workbookView xWindow="3504" yWindow="1212" windowWidth="17916" windowHeight="11256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Category</t>
   </si>
@@ -32,28 +39,31 @@
     <t>Transportation</t>
   </si>
   <si>
-    <t>Bills</t>
-  </si>
-  <si>
     <t>Food</t>
-  </si>
-  <si>
-    <t>Clothing</t>
   </si>
   <si>
     <t>Other</t>
   </si>
   <si>
-    <t>Housing</t>
+    <t>Total</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Housing/
+Utilities</t>
+  </si>
+  <si>
+    <t>Insurance/
+Medical</t>
+  </si>
+  <si>
+    <t>Saving/Giving/
+Paying off Debt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,11 +128,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,7 +174,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -231,25 +254,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>535305</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>573405</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>121921</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2876550" y="1419225"/>
-          <a:ext cx="5295900" cy="457200"/>
+          <a:off x="3674745" y="952501"/>
+          <a:ext cx="5433060" cy="632460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -296,7 +325,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> any expenses for the categories below.  Feel free to modify or add categories based on your budget.  </a:t>
+            <a:t> any expenses for the categories below.  Feel free to modify or add categories based on your budget.  Make sure to enter at least 10 items and make sure that at least three categories have more then one item.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -569,84 +598,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="7" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="str">
+        <f>B11</f>
+        <v>Housing/
+Utilities</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="str">
+        <f>C11</f>
+        <v>Transportation</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="str">
+        <f>D11</f>
+        <v>Food</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="str">
+        <f>E11</f>
+        <v>Insurance/
+Medical</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="str">
+        <f>F11</f>
+        <v>Other</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="str">
+        <f>G11</f>
+        <v>Saving/Giving/
+Paying off Debt</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -654,7 +692,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -662,7 +700,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -670,7 +708,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -678,7 +716,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -686,7 +724,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -694,7 +732,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -702,7 +740,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -710,7 +748,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -718,7 +756,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -726,7 +764,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -734,7 +772,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -742,7 +780,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -750,301 +788,301 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed wording on instructions
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
+++ b/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\Offline\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF973B77-54C8-4AED-A240-BF1CC3A75B58}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93EE87D-A5B7-4E53-A0F6-7D12A611652C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3504" yWindow="1212" windowWidth="17916" windowHeight="11256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Category</t>
   </si>
@@ -254,15 +254,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>535305</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>60961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>573405</xdr:colOff>
+      <xdr:colOff>306705</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>121921</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -277,8 +277,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3674745" y="952501"/>
-          <a:ext cx="5433060" cy="632460"/>
+          <a:off x="3337560" y="1158241"/>
+          <a:ext cx="5503545" cy="480059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -325,7 +325,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> any expenses for the categories below.  Feel free to modify or add categories based on your budget.  Make sure to enter at least 10 items and make sure that at least three categories have more then one item.</a:t>
+            <a:t> expenses for the categories below for a typical month.  Make sure to enter at least 10 items and make sure that at least three categories have more then one item.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -602,7 +602,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added a bit to make it more like the ma
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
+++ b/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\Offline\Course Materials\git\Teaching\144F20\Topic 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21809FF7-56DB-4A8E-A002-5816279CAA03}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{21809FF7-56DB-4A8E-A002-5816279CAA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CBA7B67C-7484-4D59-BD89-36B97AC0AA94}"/>
   <bookViews>
-    <workbookView xWindow="1764" yWindow="492" windowWidth="17916" windowHeight="11256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2352" windowWidth="20316" windowHeight="10152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Category</t>
   </si>
@@ -103,7 +105,14 @@
   </si>
   <si>
     <t>2.  Enter a formula in each cell of column B to compute the total spent for each category. Use the =SUM(DATA) formula. Make sure to format as currency with two decimal places.
-3.  Then create a pie chart based on these totals. Make sure that the pie chart shows the percentages of your total budget. Remove the legend and change the title.</t>
+3.  Add a pie chart based on these totals. Make sure that the pie chart shows the percentages of your total budget. Make sure the categories are labeled and set the title.
+4. Add a bar chart showing the totals, set the axis label and title.</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>Percent of total</t>
   </si>
 </sst>
 </file>
@@ -179,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -203,32 +212,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -322,25 +305,111 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -348,47 +417,73 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -396,24 +491,13 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -421,32 +505,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -454,81 +609,19 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -810,269 +903,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.109375" customWidth="1"/>
     <col min="2" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="9" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="str">
+      <c r="B1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="36" t="str">
         <f>B11</f>
         <v>Housing/
 Utilities</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="str">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="37" t="str">
         <f>C11</f>
         <v>Transportation</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="5" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="str">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="37" t="str">
         <f>D11</f>
         <v>Food</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="36" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="str">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="str">
         <f>E11</f>
         <v>Insurance/
 Medical</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="35" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="34"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="str">
+      <c r="I5" s="26"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="str">
         <f>F11</f>
         <v>Other</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="G6" s="8" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="str">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="str">
         <f>G11</f>
         <v>Saving/Giving/
 Paying off Debt</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="G7" s="10" t="s">
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G8" s="12" t="s">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="H8" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="28" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="13" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="H9" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="I9" s="30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="14" t="s">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="H10" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="I10" s="34" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
@@ -1372,13 +1487,13 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C2:F5"/>
     <mergeCell ref="C9:F10"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="D2:G7"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{1DE907B6-307C-42D2-B4E3-982D6AFCB219}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{53D464FC-793C-400A-AC43-28A9D19982E4}"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{1DE907B6-307C-42D2-B4E3-982D6AFCB219}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{53D464FC-793C-400A-AC43-28A9D19982E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>

</xml_diff>

<commit_message>
added instructions and example
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
+++ b/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{21809FF7-56DB-4A8E-A002-5816279CAA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CBA7B67C-7484-4D59-BD89-36B97AC0AA94}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{21809FF7-56DB-4A8E-A002-5816279CAA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BE05FFAB-3E8D-478B-A2FC-7938402CC3FE}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2352" windowWidth="20316" windowHeight="10152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2568" yWindow="1332" windowWidth="19668" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Category</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Video on formatting</t>
   </si>
   <si>
-    <t>1. Enter expenses for the categories below for a typical month.  Make sure to enter at least 10 items and make sure that at least three categories have more then one item.</t>
-  </si>
-  <si>
     <t>Legend</t>
   </si>
   <si>
@@ -102,24 +99,33 @@
   </si>
   <si>
     <t>Video on Pie Chart</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>Percent of total</t>
   </si>
   <si>
     <t>2.  Enter a formula in each cell of column B to compute the total spent for each category. Use the =SUM(DATA) formula. Make sure to format as currency with two decimal places.
 3.  Add a pie chart based on these totals. Make sure that the pie chart shows the percentages of your total budget. Make sure the categories are labeled and set the title.
-4. Add a bar chart showing the totals, set the axis label and title.</t>
-  </si>
-  <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
-    <t>Percent of total</t>
+4. Add a bar chart showing the subtotals, set the axis label and title.</t>
+  </si>
+  <si>
+    <t>1. Enter expenses for the categories below for a typical month.  Make sure to enter at least 10 items and make sure that at least three categories have more than one item.</t>
+  </si>
+  <si>
+    <t>Make sure to format dollar amounts as currency with two decimal places, like $12.45, and percentages with two decimals, like 1.23%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +148,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Comic Sans MS"/>
+      <family val="4"/>
     </font>
   </fonts>
   <fills count="8">
@@ -188,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -495,6 +507,56 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -505,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -521,65 +583,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -622,6 +631,74 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -906,7 +983,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,155 +995,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>24</v>
+      <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="str">
+      <c r="A2" s="19" t="str">
         <f>B11</f>
         <v>Housing/
 Utilities</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
+      <c r="B2" s="36">
+        <f>SUM(B12:B24)</f>
+        <v>1530</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="str">
+      <c r="A3" s="20" t="str">
         <f>C11</f>
         <v>Transportation</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
       <c r="H3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="37" t="str">
+      <c r="A4" s="20" t="str">
         <f>D11</f>
         <v>Food</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="str">
+      <c r="A5" s="20" t="str">
         <f>E11</f>
         <v>Insurance/
 Medical</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="26"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="str">
+      <c r="A6" s="20" t="str">
         <f>F11</f>
         <v>Other</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="27" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="28" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="str">
+      <c r="A7" s="21" t="str">
         <f>G11</f>
         <v>Saving/Giving/
 Paying off Debt</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="29" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="30" t="s">
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="H8" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="H8" s="31" t="s">
+      <c r="I8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="30" t="s">
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="H9" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-      <c r="H9" s="32" t="s">
+      <c r="I9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="30" t="s">
+    </row>
+    <row r="10" spans="1:9" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
+      <c r="H10" s="16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
-      <c r="H10" s="33" t="s">
+      <c r="I10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+    </row>
+    <row r="11" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="47"/>
+      <c r="B11" s="37" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1085,32 +1169,40 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
+    <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="47"/>
+      <c r="B12" s="38">
+        <v>1500</v>
+      </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="5"/>
+    <row r="13" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="47"/>
+      <c r="B13" s="38">
+        <v>30</v>
+      </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="5"/>
+    <row r="14" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="47"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="5"/>
+    <row r="15" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="48"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1486,10 +1578,11 @@
       <c r="G61" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C9:F10"/>
     <mergeCell ref="D2:G7"/>
     <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A10:A15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1" xr:uid="{1DE907B6-307C-42D2-B4E3-982D6AFCB219}"/>

</xml_diff>

<commit_message>
Added video on range
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
+++ b/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{21809FF7-56DB-4A8E-A002-5816279CAA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{886284BC-DCB5-4DF6-9135-24A5B448A4DC}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{21809FF7-56DB-4A8E-A002-5816279CAA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32964023-7DA1-4B68-BE48-55BAF852D1CE}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="22188" windowHeight="11508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t>Video on Pie Chart</t>
   </si>
   <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
     <t>Percent of total</t>
   </si>
   <si>
@@ -178,6 +175,31 @@
   </si>
   <si>
     <t>Video on bar chart</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Subtotal</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Video on this</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -187,7 +209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +251,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -624,7 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -640,9 +670,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -678,9 +705,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
@@ -694,6 +718,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -732,7 +757,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1017,7 +1050,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D1" sqref="D1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,173 +1062,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="D1" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="str">
+      <c r="A2" s="17" t="str">
         <f>B11</f>
         <v>Housing/
 Utilities</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="23">
         <f>SUM(B12:B24)</f>
         <v>1530</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41" t="s">
-        <v>26</v>
+      <c r="C2" s="20"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="27" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="str">
+      <c r="A3" s="18" t="str">
         <f>C11</f>
         <v>Transportation</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="str">
+      <c r="A4" s="18" t="str">
         <f>D11</f>
         <v>Food</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
       <c r="H4" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="str">
+      <c r="A5" s="18" t="str">
         <f>E11</f>
         <v>Insurance/
 Medical</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="35" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="36"/>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="str">
+      <c r="A6" s="18" t="str">
         <f>F11</f>
         <v>Other</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="10" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="str">
+      <c r="A7" s="19" t="str">
         <f>G11</f>
         <v>Saving/Giving/
 Paying off Debt</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="12" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="14" t="s">
+      <c r="B8" s="7"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
+      <c r="H9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
-      <c r="H9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
-      <c r="H10" s="16" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="H10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="37"/>
+      <c r="B11" s="24" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1215,8 +1248,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="27">
+      <c r="A12" s="37"/>
+      <c r="B12" s="25">
         <v>1500</v>
       </c>
       <c r="C12" s="5"/>
@@ -1226,8 +1259,8 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
-      <c r="B13" s="27">
+      <c r="A13" s="37"/>
+      <c r="B13" s="25">
         <v>30</v>
       </c>
       <c r="C13" s="5"/>
@@ -1237,8 +1270,8 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1246,8 +1279,8 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="39"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1633,9 +1666,10 @@
     <hyperlink ref="H3" r:id="rId1" xr:uid="{1DE907B6-307C-42D2-B4E3-982D6AFCB219}"/>
     <hyperlink ref="H4" r:id="rId2" xr:uid="{53D464FC-793C-400A-AC43-28A9D19982E4}"/>
     <hyperlink ref="H2" r:id="rId3" xr:uid="{04C1791B-DA4E-4034-BEAE-75DA9F7EA87A}"/>
+    <hyperlink ref="B1" r:id="rId4" display="https://www.loom.com/share/85a3f365a36b44268ad7bdd7904df6e2" xr:uid="{D7CABF90-EB57-41A7-8BD2-DD2E42A00666}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved videos to YouTube
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
+++ b/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{21809FF7-56DB-4A8E-A002-5816279CAA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0E341806-A57E-49DE-B49F-FDA4BB9A0187}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{21809FF7-56DB-4A8E-A002-5816279CAA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FAA2DB37-91BF-47AF-9D0E-0B04A112290A}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1680" windowWidth="15900" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Category</t>
   </si>
@@ -177,29 +177,11 @@
     <t>Video on bar chart</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Subtotal</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t>(silent video)</t>
+  </si>
+  <si>
+    <t>Subtotal
 Video on this</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -254,6 +236,7 @@
     </font>
     <font>
       <b/>
+      <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -694,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -743,6 +726,24 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -760,33 +761,41 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -797,38 +806,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1114,7 +1100,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,21 +1112,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="49" t="s">
+      <c r="B1" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:9" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="str">
@@ -1153,11 +1139,11 @@
         <v>1530</v>
       </c>
       <c r="C2" s="16"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="31" t="s">
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="50" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1168,12 +1154,15 @@
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="32" t="s">
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="51" t="s">
         <v>8</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1183,11 +1172,11 @@
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="32" t="s">
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="51" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1199,14 +1188,14 @@
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="33" t="s">
+      <c r="D5" s="39"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="29"/>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="str">
@@ -1215,11 +1204,11 @@
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="34" t="s">
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="23" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="8" t="s">
@@ -1234,11 +1223,11 @@
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="35" t="s">
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="9" t="s">
@@ -1250,11 +1239,11 @@
         <v>4</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="36" t="s">
+      <c r="D8" s="42"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="25" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="9" t="s">
@@ -1278,25 +1267,25 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
     </row>
     <row r="12" spans="1:9" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
+      <c r="A12" s="46"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="20" t="s">
         <v>5</v>
       </c>
@@ -1317,7 +1306,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="21">
         <v>1500</v>
       </c>
@@ -1328,7 +1317,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="21">
         <v>30</v>
       </c>
@@ -1339,7 +1328,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="22"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1348,7 +1337,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="22"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1719,7 +1708,7 @@
     <hyperlink ref="H3" r:id="rId1" xr:uid="{1DE907B6-307C-42D2-B4E3-982D6AFCB219}"/>
     <hyperlink ref="H4" r:id="rId2" xr:uid="{53D464FC-793C-400A-AC43-28A9D19982E4}"/>
     <hyperlink ref="H2" r:id="rId3" xr:uid="{04C1791B-DA4E-4034-BEAE-75DA9F7EA87A}"/>
-    <hyperlink ref="B1" r:id="rId4" display="https://www.loom.com/share/85a3f365a36b44268ad7bdd7904df6e2" xr:uid="{D7CABF90-EB57-41A7-8BD2-DD2E42A00666}"/>
+    <hyperlink ref="B1" r:id="rId4" display="https://youtu.be/ZshkslP__Hs" xr:uid="{D7CABF90-EB57-41A7-8BD2-DD2E42A00666}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>

</xml_diff>

<commit_message>
added vid for online Excel
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
+++ b/144F20/Topic 2/QR_2-2_Tech_Template.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcumail-my.sharepoint.com/personal/richard_ketchersid_gcu_edu/Documents/Course Materials/git/Teaching/144F20/Topic 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="10_ncr:80_{D3452BF7-3F29-44F5-913C-BD3C08EBFBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D91D724-0DED-4DCC-ADD2-673C979EC12E}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="10_ncr:80_{D3452BF7-3F29-44F5-913C-BD3C08EBFBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CC82686-AA8C-4D12-A388-C600F83B590B}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="19272" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="20796" windowHeight="11424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
     <sheet name="Bar Chart" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="Ignore Halo" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="Richard Ketchersid - Personal View" guid="{D46CCC17-9CFA-490D-812B-BC1D3CD69288}" mergeInterval="0" personalView="1" xWindow="59" yWindow="37" windowWidth="1706" windowHeight="935" activeSheetId="1"/>
@@ -99,7 +96,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -121,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Category</t>
   </si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>Values</t>
+  </si>
+  <si>
+    <t>Charts using online Excel</t>
   </si>
 </sst>
 </file>
@@ -762,7 +762,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -887,113 +887,121 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4215,89 +4223,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Housing/
-Utilities</v>
-          </cell>
-          <cell r="B3">
-            <v>1590</v>
-          </cell>
-          <cell r="C3">
-            <v>0.62970297029702971</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Transportation</v>
-          </cell>
-          <cell r="B4">
-            <v>250</v>
-          </cell>
-          <cell r="C4">
-            <v>9.9009900990099015E-2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Food</v>
-          </cell>
-          <cell r="B5">
-            <v>205</v>
-          </cell>
-          <cell r="C5">
-            <v>8.1188118811881191E-2</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Insurance/
-Medical</v>
-          </cell>
-          <cell r="B6">
-            <v>200</v>
-          </cell>
-          <cell r="C6">
-            <v>7.9207920792079209E-2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Other</v>
-          </cell>
-          <cell r="B7">
-            <v>100</v>
-          </cell>
-          <cell r="C7">
-            <v>3.9603960396039604E-2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Saving/Giving/
-Paying off Debt</v>
-          </cell>
-          <cell r="B8">
-            <v>180</v>
-          </cell>
-          <cell r="C8">
-            <v>7.1287128712871281E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4561,7 +4486,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -4575,8 +4500,8 @@
     <col min="9" max="9" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:9" ht="16.8" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="34" t="s">
         <v>27</v>
       </c>
@@ -4584,8 +4509,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -4595,18 +4520,18 @@
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="59" t="s">
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="60"/>
-    </row>
-    <row r="5" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="63"/>
+    </row>
+    <row r="5" spans="1:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="str">
         <f>B17</f>
         <v>Housing/
@@ -4617,26 +4542,29 @@
         <v>1530</v>
       </c>
       <c r="C5" s="16"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="66"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="str">
         <f>C17</f>
         <v>Transportation</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="46"/>
       <c r="H6" s="20" t="s">
         <v>8</v>
       </c>
@@ -4644,23 +4572,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="str">
         <f>D17</f>
         <v>Food</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="46"/>
       <c r="H7" s="22" t="s">
         <v>20</v>
       </c>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="str">
         <f>E17</f>
         <v>Insurance/
@@ -4668,26 +4596,26 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="36" t="s">
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="37"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I8" s="40"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="str">
         <f>F17</f>
         <v>Other</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="43"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="46"/>
       <c r="H9" s="7" t="s">
         <v>10</v>
       </c>
@@ -4695,7 +4623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="str">
         <f>G17</f>
         <v>Saving/Giving/
@@ -4703,10 +4631,10 @@
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="43"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="46"/>
       <c r="H10" s="8" t="s">
         <v>12</v>
       </c>
@@ -4714,16 +4642,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="46"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="49"/>
       <c r="H11" s="9" t="s">
         <v>14</v>
       </c>
@@ -4731,7 +4659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -4746,7 +4674,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -4761,43 +4689,43 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
+    <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="50" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="13"/>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="52"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="55"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="48"/>
+    <row r="15" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="51"/>
       <c r="B15" s="13"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="58"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="48"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
+    <row r="16" spans="1:10" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="51"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="61"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="27" t="s">
         <v>5</v>
       </c>
@@ -4820,7 +4748,7 @@
       <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="31">
         <v>1500</v>
       </c>
@@ -4833,7 +4761,7 @@
       <c r="I18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="31">
         <v>30</v>
       </c>
@@ -4846,7 +4774,7 @@
       <c r="I19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="49"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="33"/>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
@@ -5236,7 +5164,7 @@
       <c r="G64" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="moZAHjZIeW12C3nkQyiwj0PDu102o0BQAQSZfEzUSjntceTk9oJX11jKhPjCdDz/mXkQ/yDhQ+ocJm0pi7bDRA==" saltValue="7BgtWrWo80/1d7qqs726ZA==" spinCount="100000" sheet="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0"/>
   <customSheetViews>
     <customSheetView guid="{D46CCC17-9CFA-490D-812B-BC1D3CD69288}">
       <selection activeCell="B3" sqref="B3"/>
@@ -5244,12 +5172,13 @@
       <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="D4:G11"/>
     <mergeCell ref="A14:A20"/>
     <mergeCell ref="C14:F16"/>
     <mergeCell ref="H4:I4"/>
+    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:I30 A4:H4">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -5262,10 +5191,11 @@
     <hyperlink ref="H5" r:id="rId4" xr:uid="{04C1791B-DA4E-4034-BEAE-75DA9F7EA87A}"/>
     <hyperlink ref="B4" r:id="rId5" display="https://youtu.be/ZshkslP__Hs" xr:uid="{D7CABF90-EB57-41A7-8BD2-DD2E42A00666}"/>
     <hyperlink ref="H4:I4" r:id="rId6" display="Video for adding elements to charts for MAC users." xr:uid="{1F0D7A9E-34E4-4C03-A4EC-DA5B7B714AFB}"/>
+    <hyperlink ref="I5:J5" r:id="rId7" display="Charts using online Excel" xr:uid="{C4930F6B-9A6C-4A38-BDF0-96E3AECC9FCC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -5283,10 +5213,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="38" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5294,11 +5224,11 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="62" cm="1">
+      <c r="B3" s="36" cm="1">
         <f t="array" ref="B3:B8">Budget!B5:B10</f>
         <v>1530</v>
       </c>
-      <c r="C3" s="63" cm="1">
+      <c r="C3" s="37" cm="1">
         <f t="array" ref="C3:C8">_xlfn.ANCHORARRAY(B3)/B9</f>
         <v>1</v>
       </c>
@@ -5307,10 +5237,10 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="62">
+      <c r="B4" s="36">
         <v>0</v>
       </c>
-      <c r="C4" s="63">
+      <c r="C4" s="37">
         <v>0</v>
       </c>
     </row>
@@ -5318,10 +5248,10 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="62">
+      <c r="B5" s="36">
         <v>0</v>
       </c>
-      <c r="C5" s="63">
+      <c r="C5" s="37">
         <v>0</v>
       </c>
     </row>
@@ -5329,10 +5259,10 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="62">
+      <c r="B6" s="36">
         <v>0</v>
       </c>
-      <c r="C6" s="63">
+      <c r="C6" s="37">
         <v>0</v>
       </c>
     </row>
@@ -5340,10 +5270,10 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="62">
+      <c r="B7" s="36">
         <v>0</v>
       </c>
-      <c r="C7" s="63">
+      <c r="C7" s="37">
         <v>0</v>
       </c>
     </row>
@@ -5351,15 +5281,15 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="62">
+      <c r="B8" s="36">
         <v>0</v>
       </c>
-      <c r="C8" s="63">
+      <c r="C8" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="62">
+      <c r="B9" s="36">
         <f>SUM(B3:B8)</f>
         <v>1530</v>
       </c>
@@ -5382,62 +5312,62 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="4" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
     </row>
   </sheetData>
   <customSheetViews>

</xml_diff>